<commit_message>
Updates to wording and downloadable data.
</commit_message>
<xml_diff>
--- a/downloads/Induced-Travel-Calculator-Data.xlsx
+++ b/downloads/Induced-Travel-Calculator-Data.xlsx
@@ -1,14 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887C4950-1FC4-3E43-890C-FADCF0802BAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmvolker/Desktop/Professional/Post Doc/Induced VMT Calculator/Calculator Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C51437-0578-B24B-8B20-ED542DBA4DA6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="1060" windowWidth="24060" windowHeight="15200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="28800" windowHeight="16680" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2016 Data" sheetId="7" r:id="rId1"/>
+    <sheet name="2019" sheetId="8" r:id="rId1"/>
+    <sheet name="2018" sheetId="6" r:id="rId2"/>
+    <sheet name="2017" sheetId="7" r:id="rId3"/>
+    <sheet name="2016" sheetId="9" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -20,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="68">
   <si>
     <t>ALAMEDA</t>
   </si>
@@ -196,6 +204,9 @@
     <t>YUBA</t>
   </si>
   <si>
+    <t>County</t>
+  </si>
+  <si>
     <t xml:space="preserve">Interstate (Class 1) Lane Miles </t>
   </si>
   <si>
@@ -205,22 +216,31 @@
     <t>Class 3 Facility Lane Miles</t>
   </si>
   <si>
+    <t>Interstate (Class 1) Annual VMT (millions)</t>
+  </si>
+  <si>
+    <t>Class 2 Facility Annual VMT (millions)</t>
+  </si>
+  <si>
+    <t>Class 3 Facility Annual VMT (millions)</t>
+  </si>
+  <si>
+    <t>Interstate (Class 1) Auto VMT (millions)</t>
+  </si>
+  <si>
+    <t>Class 2 Facility Auto VMT (millions)</t>
+  </si>
+  <si>
     <t>Class 3 Facility Auto VMT (millions)</t>
-  </si>
-  <si>
-    <t>Class 2 Facility Auto VMT (millions)</t>
-  </si>
-  <si>
-    <t>Interstate (Class 1) Auto VMT (millions)</t>
-  </si>
-  <si>
-    <t>NOTE: All data from 2016</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -238,12 +258,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -273,16 +299,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -347,9 +378,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -382,9 +413,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -563,43 +594,1223 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86AFF54D-644F-E540-84BD-3AFB436569EA}">
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.83203125" customWidth="1"/>
+    <col min="5" max="5" width="36.5" customWidth="1"/>
+    <col min="6" max="6" width="29" customWidth="1"/>
+    <col min="7" max="7" width="36.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1007.54</v>
+      </c>
+      <c r="C2" s="6">
+        <v>136.77000000000001</v>
+      </c>
+      <c r="D2" s="6">
+        <v>838.57</v>
+      </c>
+      <c r="E2" s="6">
+        <v>7808.58</v>
+      </c>
+      <c r="F2" s="6">
+        <v>846.51</v>
+      </c>
+      <c r="G2" s="6">
+        <v>2299.86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6">
+        <v>53.01</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6">
+        <v>28.59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6">
+        <v>215.8</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6">
+        <v>255.36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6">
+        <v>15.11</v>
+      </c>
+      <c r="D5" s="6">
+        <v>344.47</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6">
+        <v>37.520000000000003</v>
+      </c>
+      <c r="G5" s="6">
+        <v>841.41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6">
+        <v>96.78</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6">
+        <v>110.05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6">
+        <v>138.55000000000001</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6">
+        <v>90.78</v>
+      </c>
+      <c r="E7" s="6">
+        <v>392.97</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6">
+        <v>108.02</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6">
+        <v>379.83</v>
+      </c>
+      <c r="C8" s="6">
+        <v>299.67</v>
+      </c>
+      <c r="D8" s="6">
+        <v>766.77</v>
+      </c>
+      <c r="E8" s="6">
+        <v>2668.9</v>
+      </c>
+      <c r="F8" s="6">
+        <v>1946.11</v>
+      </c>
+      <c r="G8" s="6">
+        <v>1950.67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6">
+        <v>204.54</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6">
+        <v>180.51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6">
+        <v>79.33</v>
+      </c>
+      <c r="D10" s="6">
+        <v>225.49</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6">
+        <v>421.3</v>
+      </c>
+      <c r="G10" s="6">
+        <v>417.11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6">
+        <v>264.64</v>
+      </c>
+      <c r="C11" s="6">
+        <v>391.49</v>
+      </c>
+      <c r="D11" s="6">
+        <v>828.52</v>
+      </c>
+      <c r="E11" s="6">
+        <v>973.35</v>
+      </c>
+      <c r="F11" s="6">
+        <v>2227.84</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1426.67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6">
+        <v>115.28</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6">
+        <v>33.520000000000003</v>
+      </c>
+      <c r="E12" s="6">
+        <v>294.12</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6">
+        <v>48.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6">
+        <v>656.46</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6">
+        <v>782.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6">
+        <v>375.74</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6">
+        <v>726.84</v>
+      </c>
+      <c r="E14" s="6">
+        <v>537.20000000000005</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6">
+        <v>849.44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6">
+        <v>503.84</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6">
+        <v>342.79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="6">
+        <v>394.66</v>
+      </c>
+      <c r="C16" s="6">
+        <v>777.76</v>
+      </c>
+      <c r="D16" s="6">
+        <v>1446.89</v>
+      </c>
+      <c r="E16" s="6">
+        <v>1490.4</v>
+      </c>
+      <c r="F16" s="6">
+        <v>2584</v>
+      </c>
+      <c r="G16" s="6">
+        <v>1944.62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="6">
+        <v>106.96</v>
+      </c>
+      <c r="C17" s="6">
+        <v>63.98</v>
+      </c>
+      <c r="D17" s="6">
+        <v>194.26</v>
+      </c>
+      <c r="E17" s="6">
+        <v>377.19</v>
+      </c>
+      <c r="F17" s="6">
+        <v>230.08</v>
+      </c>
+      <c r="G17" s="6">
+        <v>284.05</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6">
+        <v>200.18</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6">
+        <v>288.70999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6">
+        <v>406.96</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6">
+        <v>228.04</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="6">
+        <v>2827.06</v>
+      </c>
+      <c r="C20" s="6">
+        <v>1722.58</v>
+      </c>
+      <c r="D20" s="6">
+        <v>7869.29</v>
+      </c>
+      <c r="E20" s="6">
+        <v>23980.92</v>
+      </c>
+      <c r="F20" s="6">
+        <v>13467.65</v>
+      </c>
+      <c r="G20" s="6">
+        <v>16656.03</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6">
+        <v>123.91</v>
+      </c>
+      <c r="D21" s="6">
+        <v>184.07</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6">
+        <v>779.68</v>
+      </c>
+      <c r="G21" s="6">
+        <v>387.11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="6">
+        <v>25.89</v>
+      </c>
+      <c r="C22" s="6">
+        <v>235.89</v>
+      </c>
+      <c r="D22" s="6">
+        <v>83.53</v>
+      </c>
+      <c r="E22" s="6">
+        <v>166.61</v>
+      </c>
+      <c r="F22" s="6">
+        <v>1506.04</v>
+      </c>
+      <c r="G22" s="6">
+        <v>201.85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6">
+        <v>223.69</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6">
+        <v>106.33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6">
+        <v>0.99</v>
+      </c>
+      <c r="D24" s="6">
+        <v>372.29</v>
+      </c>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6">
+        <v>1.27</v>
+      </c>
+      <c r="G24" s="6">
+        <v>482.47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="6">
+        <v>128.55000000000001</v>
+      </c>
+      <c r="C25" s="6">
+        <v>186.24</v>
+      </c>
+      <c r="D25" s="6">
+        <v>406.75</v>
+      </c>
+      <c r="E25" s="6">
+        <v>462.23</v>
+      </c>
+      <c r="F25" s="6">
+        <v>750.84</v>
+      </c>
+      <c r="G25" s="6">
+        <v>706.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6">
+        <v>268.11</v>
+      </c>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6">
+        <v>64.48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6">
+        <v>465.52</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6">
+        <v>224.78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6">
+        <v>513.09</v>
+      </c>
+      <c r="D28" s="6">
+        <v>276.86</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6">
+        <v>1647.66</v>
+      </c>
+      <c r="G28" s="6">
+        <v>800.85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6">
+        <v>38.32</v>
+      </c>
+      <c r="D29" s="6">
+        <v>104.52</v>
+      </c>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6">
+        <v>166.01</v>
+      </c>
+      <c r="G29" s="6">
+        <v>308.04000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="6">
+        <v>168.61</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6">
+        <v>143.65</v>
+      </c>
+      <c r="E30" s="6">
+        <v>333.91</v>
+      </c>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6">
+        <v>312.3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="6">
+        <v>756.96</v>
+      </c>
+      <c r="C31" s="6">
+        <v>914.61</v>
+      </c>
+      <c r="D31" s="6">
+        <v>3533.79</v>
+      </c>
+      <c r="E31" s="6">
+        <v>7061.66</v>
+      </c>
+      <c r="F31" s="6">
+        <v>6200</v>
+      </c>
+      <c r="G31" s="6">
+        <v>7399.14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="6">
+        <v>337.14</v>
+      </c>
+      <c r="C32" s="6">
+        <v>43.74</v>
+      </c>
+      <c r="D32" s="6">
+        <v>260.74</v>
+      </c>
+      <c r="E32" s="6">
+        <v>1425.57</v>
+      </c>
+      <c r="F32" s="6">
+        <v>280.14</v>
+      </c>
+      <c r="G32" s="6">
+        <v>575.94000000000005</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="6">
+        <v>1385.37</v>
+      </c>
+      <c r="C34" s="6">
+        <v>353.35</v>
+      </c>
+      <c r="D34" s="6">
+        <v>1054.5</v>
+      </c>
+      <c r="E34" s="6">
+        <v>7901.44</v>
+      </c>
+      <c r="F34" s="6">
+        <v>3059.33</v>
+      </c>
+      <c r="G34" s="6">
+        <v>2447.52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="6">
+        <v>364.02</v>
+      </c>
+      <c r="C35" s="6">
+        <v>378.09</v>
+      </c>
+      <c r="D35" s="6">
+        <v>1335.19</v>
+      </c>
+      <c r="E35" s="6">
+        <v>2588.09</v>
+      </c>
+      <c r="F35" s="6">
+        <v>2927.95</v>
+      </c>
+      <c r="G35" s="6">
+        <v>3701.76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6">
+        <v>31.28</v>
+      </c>
+      <c r="D36" s="6">
+        <v>97.12</v>
+      </c>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6">
+        <v>153.96</v>
+      </c>
+      <c r="G36" s="6">
+        <v>335.07</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="6">
+        <v>2080.67</v>
+      </c>
+      <c r="C37" s="6">
+        <v>386.36</v>
+      </c>
+      <c r="D37" s="6">
+        <v>1738.72</v>
+      </c>
+      <c r="E37" s="6">
+        <v>9577.77</v>
+      </c>
+      <c r="F37" s="6">
+        <v>3090.74</v>
+      </c>
+      <c r="G37" s="6">
+        <v>3007.54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="6">
+        <v>1729</v>
+      </c>
+      <c r="C38" s="6">
+        <v>709.35</v>
+      </c>
+      <c r="D38" s="6">
+        <v>1396.31</v>
+      </c>
+      <c r="E38" s="6">
+        <v>12097.78</v>
+      </c>
+      <c r="F38" s="6">
+        <v>4723.3999999999996</v>
+      </c>
+      <c r="G38" s="6">
+        <v>3433.85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="6">
+        <v>75.5</v>
+      </c>
+      <c r="C39" s="6">
+        <v>75.430000000000007</v>
+      </c>
+      <c r="D39" s="6">
+        <v>381.35</v>
+      </c>
+      <c r="E39" s="6">
+        <v>423.5</v>
+      </c>
+      <c r="F39" s="6">
+        <v>732.25</v>
+      </c>
+      <c r="G39" s="6">
+        <v>901.27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="6">
+        <v>409.11</v>
+      </c>
+      <c r="C40" s="6">
+        <v>264.97000000000003</v>
+      </c>
+      <c r="D40" s="6">
+        <v>777.91</v>
+      </c>
+      <c r="E40" s="6">
+        <v>2149.2199999999998</v>
+      </c>
+      <c r="F40" s="6">
+        <v>1586.95</v>
+      </c>
+      <c r="G40" s="6">
+        <v>1513.04</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6">
+        <v>281.22000000000003</v>
+      </c>
+      <c r="D41" s="6">
+        <v>222.93</v>
+      </c>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6">
+        <v>1391.02</v>
+      </c>
+      <c r="G41" s="6">
+        <v>477.81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="6">
+        <v>241.7</v>
+      </c>
+      <c r="C42" s="6">
+        <v>303.69</v>
+      </c>
+      <c r="D42" s="6">
+        <v>335.36</v>
+      </c>
+      <c r="E42" s="6">
+        <v>1432.38</v>
+      </c>
+      <c r="F42" s="6">
+        <v>2606.4899999999998</v>
+      </c>
+      <c r="G42" s="6">
+        <v>961.6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6">
+        <v>400.24</v>
+      </c>
+      <c r="D43" s="6">
+        <v>331.55</v>
+      </c>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6">
+        <v>1557.15</v>
+      </c>
+      <c r="G43" s="6">
+        <v>566.1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="6">
+        <v>331.92</v>
+      </c>
+      <c r="C44" s="6">
+        <v>673.36</v>
+      </c>
+      <c r="D44" s="6">
+        <v>1682.5</v>
+      </c>
+      <c r="E44" s="6">
+        <v>2516.2800000000002</v>
+      </c>
+      <c r="F44" s="6">
+        <v>4915.1000000000004</v>
+      </c>
+      <c r="G44" s="6">
+        <v>4094.55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6">
+        <v>89.08</v>
+      </c>
+      <c r="D45" s="6">
+        <v>90.46</v>
+      </c>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6">
+        <v>584.82000000000005</v>
+      </c>
+      <c r="G45" s="6">
+        <v>221.93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46" s="6">
+        <v>289.56</v>
+      </c>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6">
+        <v>397.48</v>
+      </c>
+      <c r="E46" s="6">
+        <v>743.07</v>
+      </c>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6">
+        <v>367.99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" s="6">
+        <v>15.55</v>
+      </c>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6">
+        <v>18.96</v>
+      </c>
+      <c r="E47" s="6">
+        <v>45.97</v>
+      </c>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6">
+        <v>27.04</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" s="6">
+        <v>292.63</v>
+      </c>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6">
+        <v>220.42</v>
+      </c>
+      <c r="E48" s="6">
+        <v>428.82</v>
+      </c>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6">
+        <v>126.28</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" s="6">
+        <v>492.2</v>
+      </c>
+      <c r="C49" s="6">
+        <v>40.56</v>
+      </c>
+      <c r="D49" s="6">
+        <v>374.89</v>
+      </c>
+      <c r="E49" s="6">
+        <v>3215.8</v>
+      </c>
+      <c r="F49" s="6">
+        <v>178.43</v>
+      </c>
+      <c r="G49" s="6">
+        <v>824.42</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6">
+        <v>259.99</v>
+      </c>
+      <c r="D50" s="6">
+        <v>210.17</v>
+      </c>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6">
+        <v>1480.27</v>
+      </c>
+      <c r="G50" s="6">
+        <v>616.26</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51" s="6">
+        <v>113.73</v>
+      </c>
+      <c r="C51" s="6">
+        <v>150.09</v>
+      </c>
+      <c r="D51" s="6">
+        <v>408.22</v>
+      </c>
+      <c r="E51" s="6">
+        <v>481.44</v>
+      </c>
+      <c r="F51" s="6">
+        <v>1127.8900000000001</v>
+      </c>
+      <c r="G51" s="6">
+        <v>913.06</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6">
+        <v>76.180000000000007</v>
+      </c>
+      <c r="D52" s="6">
+        <v>140.44</v>
+      </c>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6">
+        <v>237.93</v>
+      </c>
+      <c r="G52" s="6">
+        <v>289.86</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53" s="6">
+        <v>164.2</v>
+      </c>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6">
+        <v>69.72</v>
+      </c>
+      <c r="E53" s="6">
+        <v>522.25</v>
+      </c>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6">
+        <v>130.24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6">
+        <v>154.87</v>
+      </c>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6">
+        <v>83.08</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6">
+        <v>308.43</v>
+      </c>
+      <c r="D55" s="6">
+        <v>435.79</v>
+      </c>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6">
+        <v>1486.9</v>
+      </c>
+      <c r="G55" s="6">
+        <v>659.33</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6">
+        <v>188.48</v>
+      </c>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6">
+        <v>234.96</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6">
+        <v>441.24</v>
+      </c>
+      <c r="D57" s="6">
+        <v>895.16</v>
+      </c>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6">
+        <v>2971.21</v>
+      </c>
+      <c r="G57" s="6">
+        <v>1593.87</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B58" s="6">
+        <v>299.56</v>
+      </c>
+      <c r="C58" s="6">
+        <v>46.84</v>
+      </c>
+      <c r="D58" s="6">
+        <v>113.56</v>
+      </c>
+      <c r="E58" s="6">
+        <v>1221.1300000000001</v>
+      </c>
+      <c r="F58" s="6">
+        <v>110.77</v>
+      </c>
+      <c r="G58" s="6">
+        <v>142.71</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6">
+        <v>48.84</v>
+      </c>
+      <c r="D59" s="6">
+        <v>103.64</v>
+      </c>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6">
+        <v>135.25</v>
+      </c>
+      <c r="G59" s="6">
+        <v>269.99</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C35FE0A-CBC4-4091-9A52-9965F92EC68C}">
+  <dimension ref="A1:G59"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="30.83203125" customWidth="1"/>
-    <col min="6" max="6" width="28.1640625" customWidth="1"/>
-    <col min="7" max="7" width="27.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.1640625" customWidth="1"/>
+    <col min="3" max="3" width="26.83203125" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" customWidth="1"/>
+    <col min="5" max="5" width="41.5" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" customWidth="1"/>
+    <col min="7" max="7" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="B1" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>62</v>
-      </c>
       <c r="G1" s="4" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -607,22 +1818,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="5">
-        <v>953.33900000000062</v>
+        <v>1008.0829999999992</v>
       </c>
       <c r="C2" s="5">
-        <v>128.57999999999998</v>
+        <v>134.19199999999995</v>
       </c>
       <c r="D2" s="5">
-        <v>836.89299999999912</v>
+        <v>867.7189999999996</v>
       </c>
       <c r="E2" s="5">
-        <v>7930.3680000000004</v>
+        <v>7801.0640000000021</v>
       </c>
       <c r="F2" s="5">
-        <v>786.41199999999981</v>
+        <v>833.88900000000001</v>
       </c>
       <c r="G2" s="5">
-        <v>2158.7280000000032</v>
+        <v>2095.4269999999956</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -632,12 +1843,12 @@
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5">
-        <v>53.007999999999996</v>
+        <v>53.008000000000017</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5">
-        <v>27.364999999999998</v>
+        <v>27.488000000000007</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -647,12 +1858,12 @@
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5">
-        <v>204.69300000000007</v>
+        <v>205.2440000000002</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5">
-        <v>233.10299999999984</v>
+        <v>233.07699999999997</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -661,17 +1872,17 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5">
-        <v>15.105999999999998</v>
+        <v>15.106</v>
       </c>
       <c r="D5" s="5">
-        <v>316.94700000000006</v>
+        <v>347.3490000000001</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5">
-        <v>34.900999999999996</v>
+        <v>37.515000000000001</v>
       </c>
       <c r="G5" s="5">
-        <v>823.68299999999931</v>
+        <v>811.2569999999987</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -681,12 +1892,12 @@
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5">
-        <v>97.64</v>
+        <v>96.777999999999992</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5">
-        <v>104.50999999999998</v>
+        <v>109.76200000000001</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -694,18 +1905,18 @@
         <v>5</v>
       </c>
       <c r="B7" s="5">
-        <v>138.54800000000006</v>
+        <v>138.548</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5">
-        <v>92.697999999999993</v>
+        <v>90.781000000000049</v>
       </c>
       <c r="E7" s="5">
-        <v>377.52600000000007</v>
+        <v>392.96599999999989</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5">
-        <v>103.69499999999996</v>
+        <v>102.72599999999994</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -713,22 +1924,22 @@
         <v>6</v>
       </c>
       <c r="B8" s="5">
-        <v>362.88599999999991</v>
+        <v>379.82700000000011</v>
       </c>
       <c r="C8" s="5">
-        <v>249.65800000000002</v>
+        <v>289.02899999999994</v>
       </c>
       <c r="D8" s="5">
-        <v>753.03599999999881</v>
+        <v>765.00800000000027</v>
       </c>
       <c r="E8" s="5">
-        <v>2767.4289999999974</v>
+        <v>2668.3480000000027</v>
       </c>
       <c r="F8" s="5">
-        <v>1945.7350000000015</v>
+        <v>1956.5830000000003</v>
       </c>
       <c r="G8" s="5">
-        <v>1734.4099999999967</v>
+        <v>1788.650999999996</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -738,12 +1949,12 @@
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5">
-        <v>210.44300000000007</v>
+        <v>204.59400000000011</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5">
-        <v>168.83600000000007</v>
+        <v>186.49699999999996</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -752,17 +1963,17 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5">
-        <v>79.635999999999996</v>
+        <v>79.326999999999998</v>
       </c>
       <c r="D10" s="5">
-        <v>217.69599999999988</v>
+        <v>225.52199999999993</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5">
-        <v>413.81</v>
+        <v>420.96099999999996</v>
       </c>
       <c r="G10" s="5">
-        <v>392.84499999999974</v>
+        <v>417.61199999999985</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -773,19 +1984,19 @@
         <v>264.63599999999997</v>
       </c>
       <c r="C11" s="5">
-        <v>381.97599999999971</v>
+        <v>392.14199999999977</v>
       </c>
       <c r="D11" s="5">
-        <v>792.27299999999934</v>
+        <v>827.87100000000032</v>
       </c>
       <c r="E11" s="5">
-        <v>946.8130000000001</v>
+        <v>974.00200000000007</v>
       </c>
       <c r="F11" s="5">
-        <v>2068.2869999999989</v>
+        <v>2153.9019999999996</v>
       </c>
       <c r="G11" s="5">
-        <v>1255.3139999999987</v>
+        <v>1233.5209999999986</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -793,18 +2004,18 @@
         <v>10</v>
       </c>
       <c r="B12" s="5">
-        <v>115.28399999999999</v>
+        <v>115.28399999999998</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5">
-        <v>34.054000000000009</v>
+        <v>34.053999999999995</v>
       </c>
       <c r="E12" s="5">
-        <v>288.63200000000006</v>
+        <v>294.11800000000005</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5">
-        <v>46.038999999999994</v>
+        <v>46.775999999999982</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -814,12 +2025,12 @@
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5">
-        <v>655.63000000000022</v>
+        <v>656.3449999999998</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5">
-        <v>743.72799999999972</v>
+        <v>783.08099999999968</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -827,18 +2038,18 @@
         <v>12</v>
       </c>
       <c r="B14" s="5">
-        <v>375.74000000000007</v>
+        <v>375.7399999999999</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5">
-        <v>678.86699999999939</v>
+        <v>688.42599999999914</v>
       </c>
       <c r="E14" s="5">
-        <v>570.30900000000008</v>
+        <v>544.31499999999994</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5">
-        <v>729.43900000000008</v>
+        <v>777.57199999999909</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -848,12 +2059,12 @@
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5">
-        <v>494.03100000000006</v>
+        <v>503.84300000000002</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5">
-        <v>340.28700000000021</v>
+        <v>336.53199999999993</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -861,22 +2072,22 @@
         <v>14</v>
       </c>
       <c r="B16" s="5">
-        <v>387.34000000000003</v>
+        <v>394.65800000000002</v>
       </c>
       <c r="C16" s="5">
-        <v>759.78200000000015</v>
+        <v>777.45600000000002</v>
       </c>
       <c r="D16" s="5">
-        <v>1282.1849999999997</v>
+        <v>1447.132999999995</v>
       </c>
       <c r="E16" s="5">
-        <v>1344.2920000000004</v>
+        <v>1409.3989999999994</v>
       </c>
       <c r="F16" s="5">
-        <v>2405.3740000000003</v>
+        <v>2563.4649999999988</v>
       </c>
       <c r="G16" s="5">
-        <v>1894.1219999999978</v>
+        <v>1694.7079999999985</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -887,19 +2098,19 @@
         <v>106.95599999999999</v>
       </c>
       <c r="C17" s="5">
-        <v>65.923000000000016</v>
+        <v>66.376000000000005</v>
       </c>
       <c r="D17" s="5">
-        <v>191.55800000000011</v>
+        <v>191.85800000000015</v>
       </c>
       <c r="E17" s="5">
-        <v>355.72500000000002</v>
+        <v>372.87900000000002</v>
       </c>
       <c r="F17" s="5">
-        <v>202.48700000000002</v>
+        <v>226.50300000000001</v>
       </c>
       <c r="G17" s="5">
-        <v>253.375</v>
+        <v>261.79500000000007</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -909,12 +2120,12 @@
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5">
-        <v>149.95699999999991</v>
+        <v>153.4200000000001</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5">
-        <v>214.08000000000004</v>
+        <v>209.88900000000001</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -924,12 +2135,12 @@
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5">
-        <v>400.71600000000024</v>
+        <v>408.49000000000018</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5">
-        <v>228.511</v>
+        <v>239.40499999999994</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -937,22 +2148,22 @@
         <v>18</v>
       </c>
       <c r="B20" s="5">
-        <v>2759.202000000002</v>
+        <v>2826.8060000000041</v>
       </c>
       <c r="C20" s="5">
-        <v>1709.853999999998</v>
+        <v>1708.3379999999988</v>
       </c>
       <c r="D20" s="5">
-        <v>7488.8019999999369</v>
+        <v>7926.4019999999728</v>
       </c>
       <c r="E20" s="5">
-        <v>23603.734999999997</v>
+        <v>23879.479000000007</v>
       </c>
       <c r="F20" s="5">
-        <v>13572.466999999997</v>
+        <v>13657.708000000017</v>
       </c>
       <c r="G20" s="5">
-        <v>19093.756999999998</v>
+        <v>17043.248000000043</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -961,17 +2172,17 @@
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5">
-        <v>123.24600000000002</v>
+        <v>123.91099999999997</v>
       </c>
       <c r="D21" s="5">
-        <v>182.68100000000007</v>
+        <v>184.14400000000003</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5">
-        <v>690.00199999999995</v>
+        <v>775.4860000000001</v>
       </c>
       <c r="G21" s="5">
-        <v>359.91500000000036</v>
+        <v>375.41400000000004</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -979,22 +2190,22 @@
         <v>20</v>
       </c>
       <c r="B22" s="5">
-        <v>27.192</v>
+        <v>25.887999999999998</v>
       </c>
       <c r="C22" s="5">
-        <v>229.75199999999995</v>
+        <v>235.89399999999995</v>
       </c>
       <c r="D22" s="5">
-        <v>92.374000000000024</v>
+        <v>90.231000000000023</v>
       </c>
       <c r="E22" s="5">
-        <v>175.50500000000002</v>
+        <v>166.613</v>
       </c>
       <c r="F22" s="5">
-        <v>1502.0050000000003</v>
+        <v>1520.5920000000003</v>
       </c>
       <c r="G22" s="5">
-        <v>218.84400000000005</v>
+        <v>201.32599999999994</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1004,12 +2215,12 @@
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5">
-        <v>201.43399999999988</v>
+        <v>223.68699999999998</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5">
-        <v>90.385999999999939</v>
+        <v>98.794999999999959</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1018,17 +2229,17 @@
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5">
-        <v>0.85599999999999998</v>
+        <v>0.99199999999999999</v>
       </c>
       <c r="D24" s="5">
-        <v>379.71199999999988</v>
+        <v>377.01099999999991</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5">
-        <v>1.448</v>
+        <v>1.484</v>
       </c>
       <c r="G24" s="5">
-        <v>536.66999999999985</v>
+        <v>500.12299999999999</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1036,22 +2247,22 @@
         <v>23</v>
       </c>
       <c r="B25" s="5">
-        <v>128.54799999999994</v>
+        <v>128.54799999999997</v>
       </c>
       <c r="C25" s="5">
-        <v>161.506</v>
+        <v>186.24400000000011</v>
       </c>
       <c r="D25" s="5">
-        <v>382.67999999999972</v>
+        <v>380.13199999999983</v>
       </c>
       <c r="E25" s="5">
-        <v>393.05999999999995</v>
+        <v>418.66099999999994</v>
       </c>
       <c r="F25" s="5">
-        <v>687.47699999999986</v>
+        <v>687.47699999999998</v>
       </c>
       <c r="G25" s="5">
-        <v>636.16999999999973</v>
+        <v>652.73799999999983</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1061,12 +2272,12 @@
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5">
-        <v>258.86199999999997</v>
+        <v>268.11200000000002</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5">
-        <v>53.625999999999983</v>
+        <v>62.321999999999989</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1076,12 +2287,12 @@
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5">
-        <v>428.38599999999997</v>
+        <v>465.25900000000013</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5">
-        <v>212.42299999999989</v>
+        <v>219.67799999999986</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1090,17 +2301,17 @@
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5">
-        <v>494.19700000000012</v>
+        <v>486.80299999999994</v>
       </c>
       <c r="D28" s="5">
-        <v>243.42499999999993</v>
+        <v>286.39799999999951</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5">
-        <v>1591.6020000000001</v>
+        <v>1614.742999999999</v>
       </c>
       <c r="G28" s="5">
-        <v>721.53300000000002</v>
+        <v>862.30099999999936</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1109,17 +2320,17 @@
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5">
-        <v>39.534999999999989</v>
+        <v>38.945000000000014</v>
       </c>
       <c r="D29" s="5">
-        <v>97.562000000000012</v>
+        <v>104.51899999999999</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5">
-        <v>182.16900000000004</v>
+        <v>174.72700000000003</v>
       </c>
       <c r="G29" s="5">
-        <v>298.35000000000008</v>
+        <v>283.73199999999997</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1127,18 +2338,18 @@
         <v>28</v>
       </c>
       <c r="B30" s="5">
-        <v>147.68199999999996</v>
+        <v>168.607</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5">
-        <v>143.74600000000007</v>
+        <v>143.65000000000015</v>
       </c>
       <c r="E30" s="5">
-        <v>320.73000000000008</v>
+        <v>320.26900000000006</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5">
-        <v>299.1880000000001</v>
+        <v>301.81699999999984</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1146,22 +2357,22 @@
         <v>29</v>
       </c>
       <c r="B31" s="5">
-        <v>755.87299999999982</v>
+        <v>759.40199999999982</v>
       </c>
       <c r="C31" s="5">
-        <v>900.91899999999998</v>
+        <v>914.61699999999894</v>
       </c>
       <c r="D31" s="5">
-        <v>3170.0179999999955</v>
+        <v>3524.9029999999934</v>
       </c>
       <c r="E31" s="5">
-        <v>6657.3329999999969</v>
+        <v>6682.9860000000035</v>
       </c>
       <c r="F31" s="5">
-        <v>6060.3620000000055</v>
+        <v>5980.7260000000051</v>
       </c>
       <c r="G31" s="5">
-        <v>7690.7980000000107</v>
+        <v>7386.1290000000035</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1169,22 +2380,22 @@
         <v>30</v>
       </c>
       <c r="B32" s="5">
-        <v>325.46100000000007</v>
+        <v>337.14400000000006</v>
       </c>
       <c r="C32" s="5">
-        <v>43.051000000000009</v>
+        <v>43.739000000000004</v>
       </c>
       <c r="D32" s="5">
-        <v>203.20000000000005</v>
+        <v>260.74000000000007</v>
       </c>
       <c r="E32" s="5">
-        <v>1391.7590000000002</v>
+        <v>1392.6369999999999</v>
       </c>
       <c r="F32" s="5">
-        <v>250.57099999999994</v>
+        <v>280.14000000000004</v>
       </c>
       <c r="G32" s="5">
-        <v>465.01600000000008</v>
+        <v>520.96200000000022</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1203,22 +2414,22 @@
         <v>32</v>
       </c>
       <c r="B34" s="5">
-        <v>1302.9670000000003</v>
+        <v>1372.0880000000004</v>
       </c>
       <c r="C34" s="5">
-        <v>366.99099999999993</v>
+        <v>379.45400000000001</v>
       </c>
       <c r="D34" s="5">
-        <v>964.74800000000062</v>
+        <v>1052.1380000000001</v>
       </c>
       <c r="E34" s="5">
-        <v>7035.6240000000007</v>
+        <v>7818.9770000000017</v>
       </c>
       <c r="F34" s="5">
-        <v>2931.7489999999993</v>
+        <v>3104.3609999999999</v>
       </c>
       <c r="G34" s="5">
-        <v>2265.1389999999997</v>
+        <v>2425.748</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -1226,22 +2437,22 @@
         <v>33</v>
       </c>
       <c r="B35" s="5">
-        <v>354.60000000000008</v>
+        <v>364.02100000000007</v>
       </c>
       <c r="C35" s="5">
-        <v>390.05900000000025</v>
+        <v>378.09400000000028</v>
       </c>
       <c r="D35" s="5">
-        <v>1021.3449999999982</v>
+        <v>1301.0479999999993</v>
       </c>
       <c r="E35" s="5">
-        <v>2472.2089999999998</v>
+        <v>2539.9379999999987</v>
       </c>
       <c r="F35" s="5">
-        <v>2888.7539999999985</v>
+        <v>2934.9159999999993</v>
       </c>
       <c r="G35" s="5">
-        <v>2684.3000000000034</v>
+        <v>2585.9069999999947</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -1250,17 +2461,1198 @@
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="5">
+        <v>31.277000000000001</v>
+      </c>
+      <c r="D36" s="5">
+        <v>97.06599999999996</v>
+      </c>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5">
+        <v>142.32500000000002</v>
+      </c>
+      <c r="G36" s="5">
+        <v>300.00700000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="5">
+        <v>2079.2209999999991</v>
+      </c>
+      <c r="C37" s="5">
+        <v>386.35500000000019</v>
+      </c>
+      <c r="D37" s="5">
+        <v>1799.0619999999994</v>
+      </c>
+      <c r="E37" s="5">
+        <v>9201.8960000000006</v>
+      </c>
+      <c r="F37" s="5">
+        <v>3001.5780000000022</v>
+      </c>
+      <c r="G37" s="5">
+        <v>2992.0860000000062</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="5">
+        <v>1729.1909999999978</v>
+      </c>
+      <c r="C38" s="5">
+        <v>709.83699999999942</v>
+      </c>
+      <c r="D38" s="5">
+        <v>1406.6929999999948</v>
+      </c>
+      <c r="E38" s="5">
+        <v>12106.250000000005</v>
+      </c>
+      <c r="F38" s="5">
+        <v>4618.6210000000001</v>
+      </c>
+      <c r="G38" s="5">
+        <v>3071.4429999999929</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="5">
+        <v>75.500999999999991</v>
+      </c>
+      <c r="C39" s="5">
+        <v>75.56</v>
+      </c>
+      <c r="D39" s="5">
+        <v>410.08099999999968</v>
+      </c>
+      <c r="E39" s="5">
+        <v>423.50300000000004</v>
+      </c>
+      <c r="F39" s="5">
+        <v>703.22000000000025</v>
+      </c>
+      <c r="G39" s="5">
+        <v>849.58000000000106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="5">
+        <v>409.11399999999986</v>
+      </c>
+      <c r="C40" s="5">
+        <v>259.88100000000003</v>
+      </c>
+      <c r="D40" s="5">
+        <v>779.62699999999927</v>
+      </c>
+      <c r="E40" s="5">
+        <v>2050.1250000000005</v>
+      </c>
+      <c r="F40" s="5">
+        <v>1464.7280000000005</v>
+      </c>
+      <c r="G40" s="5">
+        <v>1277.0339999999974</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5">
+        <v>281.22099999999995</v>
+      </c>
+      <c r="D41" s="5">
+        <v>234.79100000000014</v>
+      </c>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5">
+        <v>1388.6300000000003</v>
+      </c>
+      <c r="G41" s="5">
+        <v>473.06000000000017</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="5">
+        <v>241.69499999999994</v>
+      </c>
+      <c r="C42" s="5">
+        <v>327.99899999999991</v>
+      </c>
+      <c r="D42" s="5">
+        <v>278.95299999999997</v>
+      </c>
+      <c r="E42" s="5">
+        <v>1435.8680000000002</v>
+      </c>
+      <c r="F42" s="5">
+        <v>2748.502</v>
+      </c>
+      <c r="G42" s="5">
+        <v>778.73499999999967</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5">
+        <v>400.23699999999997</v>
+      </c>
+      <c r="D43" s="5">
+        <v>353.8779999999997</v>
+      </c>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5">
+        <v>1553.7700000000018</v>
+      </c>
+      <c r="G43" s="5">
+        <v>525.73799999999903</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="5">
+        <v>331.92199999999985</v>
+      </c>
+      <c r="C44" s="5">
+        <v>673.35900000000004</v>
+      </c>
+      <c r="D44" s="5">
+        <v>1671.0049999999933</v>
+      </c>
+      <c r="E44" s="5">
+        <v>2516.2939999999985</v>
+      </c>
+      <c r="F44" s="5">
+        <v>4934.5050000000019</v>
+      </c>
+      <c r="G44" s="5">
+        <v>3740.5480000000152</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5">
+        <v>125.72</v>
+      </c>
+      <c r="D45" s="5">
+        <v>97.4939999999999</v>
+      </c>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5">
+        <v>702.62100000000032</v>
+      </c>
+      <c r="G45" s="5">
+        <v>186.84600000000023</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46" s="5">
+        <v>289.55800000000005</v>
+      </c>
+      <c r="C46" s="5">
+        <v>87.000999999999962</v>
+      </c>
+      <c r="D46" s="5">
+        <v>316.44199999999995</v>
+      </c>
+      <c r="E46" s="5">
+        <v>725.45699999999908</v>
+      </c>
+      <c r="F46" s="5">
+        <v>155.30399999999997</v>
+      </c>
+      <c r="G46" s="5">
+        <v>213.16599999999991</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" s="5">
+        <v>15.548</v>
+      </c>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5">
+        <v>18.962000000000003</v>
+      </c>
+      <c r="E47" s="5">
+        <v>44.122999999999998</v>
+      </c>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5">
+        <v>18.485999999999997</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" s="5">
+        <v>292.625</v>
+      </c>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5">
+        <v>219.98800000000006</v>
+      </c>
+      <c r="E48" s="5">
+        <v>428.13299999999981</v>
+      </c>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5">
+        <v>130.40799999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" s="5">
+        <v>492.20300000000003</v>
+      </c>
+      <c r="C49" s="5">
+        <v>40.560999999999993</v>
+      </c>
+      <c r="D49" s="5">
+        <v>374.89200000000022</v>
+      </c>
+      <c r="E49" s="5">
+        <v>3219.4349999999999</v>
+      </c>
+      <c r="F49" s="5">
+        <v>167.14900000000003</v>
+      </c>
+      <c r="G49" s="5">
+        <v>681.4970000000003</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5">
+        <v>279.28699999999992</v>
+      </c>
+      <c r="D50" s="5">
+        <v>166.15900000000002</v>
+      </c>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5">
+        <v>1641.6759999999992</v>
+      </c>
+      <c r="G50" s="5">
+        <v>405.26699999999971</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51" s="5">
+        <v>113.72699999999999</v>
+      </c>
+      <c r="C51" s="5">
+        <v>150.09000000000006</v>
+      </c>
+      <c r="D51" s="5">
+        <v>408.22299999999933</v>
+      </c>
+      <c r="E51" s="5">
+        <v>482.20200000000006</v>
+      </c>
+      <c r="F51" s="5">
+        <v>966.31100000000004</v>
+      </c>
+      <c r="G51" s="5">
+        <v>819.38199999999972</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5">
+        <v>76.176999999999992</v>
+      </c>
+      <c r="D52" s="5">
+        <v>140.43499999999995</v>
+      </c>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5">
+        <v>237.24600000000007</v>
+      </c>
+      <c r="G52" s="5">
+        <v>314.2440000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53" s="5">
+        <v>164.196</v>
+      </c>
+      <c r="C53" s="5">
+        <v>6.2919999999999998</v>
+      </c>
+      <c r="D53" s="5">
+        <v>63.427000000000014</v>
+      </c>
+      <c r="E53" s="5">
+        <v>497.16899999999987</v>
+      </c>
+      <c r="F53" s="5">
+        <v>10.474</v>
+      </c>
+      <c r="G53" s="5">
+        <v>103.17400000000002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5">
+        <v>154.86500000000004</v>
+      </c>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5">
+        <v>81.256</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5">
+        <v>308.43300000000005</v>
+      </c>
+      <c r="D55" s="5">
+        <v>435.79099999999994</v>
+      </c>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5">
+        <v>1471.3670000000002</v>
+      </c>
+      <c r="G55" s="5">
+        <v>611.58199999999965</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5">
+        <v>188.47699999999995</v>
+      </c>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5">
+        <v>233.76799999999989</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5">
+        <v>429.96399999999971</v>
+      </c>
+      <c r="D57" s="5">
+        <v>921.24199999999871</v>
+      </c>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5">
+        <v>2899.344999999998</v>
+      </c>
+      <c r="G57" s="5">
+        <v>1668.3970000000006</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B58" s="5">
+        <v>298.50900000000001</v>
+      </c>
+      <c r="C58" s="5">
+        <v>47.897000000000006</v>
+      </c>
+      <c r="D58" s="5">
+        <v>119.21799999999996</v>
+      </c>
+      <c r="E58" s="5">
+        <v>1202.9729999999993</v>
+      </c>
+      <c r="F58" s="5">
+        <v>111.92600000000002</v>
+      </c>
+      <c r="G58" s="5">
+        <v>158.33999999999989</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5">
+        <v>48.835999999999991</v>
+      </c>
+      <c r="D59" s="5">
+        <v>103.63600000000001</v>
+      </c>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5">
+        <v>135.25199999999998</v>
+      </c>
+      <c r="G59" s="5">
+        <v>240.28100000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF942E30-A092-4A40-BF47-F12382A3BCC1}">
+  <dimension ref="A1:G59"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" customWidth="1"/>
+    <col min="5" max="5" width="34.83203125" customWidth="1"/>
+    <col min="6" max="6" width="30.5" customWidth="1"/>
+    <col min="7" max="7" width="30.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5">
+        <v>953.33900000000062</v>
+      </c>
+      <c r="C2" s="5">
+        <v>128.57999999999998</v>
+      </c>
+      <c r="D2" s="5">
+        <v>864.47700000000043</v>
+      </c>
+      <c r="E2" s="5">
+        <v>7930.3649999999998</v>
+      </c>
+      <c r="F2" s="5">
+        <v>786.41199999999981</v>
+      </c>
+      <c r="G2" s="5">
+        <v>2121.8710000000051</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5">
+        <v>53.007999999999996</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5">
+        <v>27.363999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5">
+        <v>204.69300000000007</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5">
+        <v>233.09499999999991</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5">
+        <v>15.105999999999998</v>
+      </c>
+      <c r="D5" s="5">
+        <v>349.55199999999996</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5">
+        <v>34.900999999999996</v>
+      </c>
+      <c r="G5" s="5">
+        <v>821.42399999999941</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5">
+        <v>97.64</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5">
+        <v>104.50599999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5">
+        <v>138.54800000000006</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5">
+        <v>92.697999999999993</v>
+      </c>
+      <c r="E7" s="5">
+        <v>377.52300000000002</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5">
+        <v>103.68999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5">
+        <v>362.88599999999991</v>
+      </c>
+      <c r="C8" s="5">
+        <v>249.65800000000002</v>
+      </c>
+      <c r="D8" s="5">
+        <v>750.40400000000045</v>
+      </c>
+      <c r="E8" s="5">
+        <v>2767.4289999999974</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1945.7350000000015</v>
+      </c>
+      <c r="G8" s="5">
+        <v>1790.1429999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5">
+        <v>210.44300000000007</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5">
+        <v>168.84900000000007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5">
+        <v>79.635999999999996</v>
+      </c>
+      <c r="D10" s="5">
+        <v>217.73199999999989</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5">
+        <v>413.81</v>
+      </c>
+      <c r="G10" s="5">
+        <v>393.09199999999981</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5">
+        <v>264.63599999999997</v>
+      </c>
+      <c r="C11" s="5">
+        <v>381.9759999999996</v>
+      </c>
+      <c r="D11" s="5">
+        <v>799.07599999999934</v>
+      </c>
+      <c r="E11" s="5">
+        <v>946.8130000000001</v>
+      </c>
+      <c r="F11" s="5">
+        <v>2068.2849999999985</v>
+      </c>
+      <c r="G11" s="5">
+        <v>1266.1080000000011</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5">
+        <v>115.28399999999999</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5">
+        <v>34.054000000000009</v>
+      </c>
+      <c r="E12" s="5">
+        <v>288.63200000000001</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5">
+        <v>46.043999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5">
+        <v>655.47200000000009</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5">
+        <v>743.60299999999984</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="5">
+        <v>375.74000000000007</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5">
+        <v>688.08599999999933</v>
+      </c>
+      <c r="E14" s="5">
+        <v>570.30400000000009</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5">
+        <v>734.34000000000049</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5">
+        <v>494.03100000000006</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5">
+        <v>340.25500000000028</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="5">
+        <v>387.34000000000003</v>
+      </c>
+      <c r="C16" s="5">
+        <v>759.78200000000015</v>
+      </c>
+      <c r="D16" s="5">
+        <v>1368.112999999998</v>
+      </c>
+      <c r="E16" s="5">
+        <v>1344.2890000000004</v>
+      </c>
+      <c r="F16" s="5">
+        <v>2405.375</v>
+      </c>
+      <c r="G16" s="5">
+        <v>1907.1119999999989</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="5">
+        <v>106.95599999999999</v>
+      </c>
+      <c r="C17" s="5">
+        <v>65.923000000000016</v>
+      </c>
+      <c r="D17" s="5">
+        <v>185.29600000000005</v>
+      </c>
+      <c r="E17" s="5">
+        <v>355.72500000000002</v>
+      </c>
+      <c r="F17" s="5">
+        <v>202.48400000000001</v>
+      </c>
+      <c r="G17" s="5">
+        <v>253.78199999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5">
+        <v>149.95699999999991</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5">
+        <v>214.07900000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5">
+        <v>400.71600000000024</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5">
+        <v>228.50500000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="5">
+        <v>2759.202000000002</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1709.8539999999982</v>
+      </c>
+      <c r="D20" s="5">
+        <v>7618.5569999999398</v>
+      </c>
+      <c r="E20" s="5">
+        <v>23670.957999999991</v>
+      </c>
+      <c r="F20" s="5">
+        <v>13572.480000000001</v>
+      </c>
+      <c r="G20" s="5">
+        <v>19199.841000000113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5">
+        <v>123.24600000000002</v>
+      </c>
+      <c r="D21" s="5">
+        <v>182.68100000000007</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5">
+        <v>690.00199999999995</v>
+      </c>
+      <c r="G21" s="5">
+        <v>360.01200000000011</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="5">
+        <v>27.192</v>
+      </c>
+      <c r="C22" s="5">
+        <v>229.75199999999995</v>
+      </c>
+      <c r="D22" s="5">
+        <v>91.072000000000031</v>
+      </c>
+      <c r="E22" s="5">
+        <v>175.50500000000002</v>
+      </c>
+      <c r="F22" s="5">
+        <v>1502.0040000000004</v>
+      </c>
+      <c r="G22" s="5">
+        <v>219.28700000000009</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5">
+        <v>201.43399999999988</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5">
+        <v>90.377999999999957</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5">
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="D24" s="5">
+        <v>379.71199999999988</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5">
+        <v>1.448</v>
+      </c>
+      <c r="G24" s="5">
+        <v>536.65999999999974</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="5">
+        <v>128.54799999999994</v>
+      </c>
+      <c r="C25" s="5">
+        <v>161.506</v>
+      </c>
+      <c r="D25" s="5">
+        <v>375.97999999999973</v>
+      </c>
+      <c r="E25" s="5">
+        <v>393.05899999999997</v>
+      </c>
+      <c r="F25" s="5">
+        <v>687.47499999999991</v>
+      </c>
+      <c r="G25" s="5">
+        <v>638.02899999999977</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5">
+        <v>258.86199999999997</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5">
+        <v>53.617999999999995</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5">
+        <v>428.38599999999997</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5">
+        <v>212.40499999999983</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5">
+        <v>494.19700000000012</v>
+      </c>
+      <c r="D28" s="5">
+        <v>254.13899999999992</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5">
+        <v>1591.5990000000002</v>
+      </c>
+      <c r="G28" s="5">
+        <v>720.09700000000032</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5">
+        <v>39.534999999999989</v>
+      </c>
+      <c r="D29" s="5">
+        <v>91.25800000000001</v>
+      </c>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5">
+        <v>182.16900000000004</v>
+      </c>
+      <c r="G29" s="5">
+        <v>274.37300000000005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="5">
+        <v>147.68199999999996</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5">
+        <v>143.74600000000007</v>
+      </c>
+      <c r="E30" s="5">
+        <v>320.72900000000004</v>
+      </c>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5">
+        <v>299.19100000000009</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="5">
+        <v>755.87299999999982</v>
+      </c>
+      <c r="C31" s="5">
+        <v>900.68799999999999</v>
+      </c>
+      <c r="D31" s="5">
+        <v>3319.5559999999932</v>
+      </c>
+      <c r="E31" s="5">
+        <v>6687.6939999999995</v>
+      </c>
+      <c r="F31" s="5">
+        <v>6059.4100000000053</v>
+      </c>
+      <c r="G31" s="5">
+        <v>7698.1000000000195</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="5">
+        <v>325.46100000000007</v>
+      </c>
+      <c r="C32" s="5">
+        <v>43.051000000000009</v>
+      </c>
+      <c r="D32" s="5">
+        <v>219.05100000000007</v>
+      </c>
+      <c r="E32" s="5">
+        <v>1391.7570000000003</v>
+      </c>
+      <c r="F32" s="5">
+        <v>250.57099999999994</v>
+      </c>
+      <c r="G32" s="5">
+        <v>475.21500000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="5">
+        <v>1302.9670000000003</v>
+      </c>
+      <c r="C34" s="5">
+        <v>366.99099999999999</v>
+      </c>
+      <c r="D34" s="5">
+        <v>1012.951000000001</v>
+      </c>
+      <c r="E34" s="5">
+        <v>7035.6200000000017</v>
+      </c>
+      <c r="F34" s="5">
+        <v>2931.7479999999991</v>
+      </c>
+      <c r="G34" s="5">
+        <v>2258.7510000000011</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="5">
+        <v>354.6</v>
+      </c>
+      <c r="C35" s="5">
+        <v>390.05900000000025</v>
+      </c>
+      <c r="D35" s="5">
+        <v>1186.8919999999991</v>
+      </c>
+      <c r="E35" s="5">
+        <v>2472.2080000000001</v>
+      </c>
+      <c r="F35" s="5">
+        <v>2888.751999999999</v>
+      </c>
+      <c r="G35" s="5">
+        <v>2579.3109999999965</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5">
         <v>25.457000000000001</v>
       </c>
       <c r="D36" s="5">
-        <v>96.586999999999961</v>
+        <v>93.06699999999995</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5">
         <v>122.58799999999999</v>
       </c>
       <c r="G36" s="5">
-        <v>245.59299999999996</v>
+        <v>245.84199999999996</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -1274,16 +3666,16 @@
         <v>383.47500000000019</v>
       </c>
       <c r="D37" s="5">
-        <v>1666.2289999999978</v>
+        <v>1710.0219999999979</v>
       </c>
       <c r="E37" s="5">
-        <v>8520.2630000000026</v>
+        <v>8520.2490000000053</v>
       </c>
       <c r="F37" s="5">
-        <v>2657.2849999999999</v>
+        <v>2657.29</v>
       </c>
       <c r="G37" s="5">
-        <v>3057.3530000000055</v>
+        <v>3074.3560000000025</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1297,16 +3689,16 @@
         <v>702.87399999999968</v>
       </c>
       <c r="D38" s="5">
-        <v>1189.8429999999978</v>
+        <v>1311.2289999999973</v>
       </c>
       <c r="E38" s="5">
-        <v>11580.371000000017</v>
+        <v>11580.43600000002</v>
       </c>
       <c r="F38" s="5">
-        <v>4741.8629999999948</v>
+        <v>4748.7349999999951</v>
       </c>
       <c r="G38" s="5">
-        <v>3139.0850000000069</v>
+        <v>3109.8680000000068</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -1320,16 +3712,16 @@
         <v>76.735000000000014</v>
       </c>
       <c r="D39" s="5">
-        <v>400.93799999999999</v>
+        <v>376.2819999999997</v>
       </c>
       <c r="E39" s="5">
-        <v>466.22399999999999</v>
+        <v>466.22200000000004</v>
       </c>
       <c r="F39" s="5">
         <v>720.48700000000031</v>
       </c>
       <c r="G39" s="5">
-        <v>981.24499999999944</v>
+        <v>983.26499999999862</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -1343,16 +3735,16 @@
         <v>248.17499999999993</v>
       </c>
       <c r="D40" s="5">
-        <v>755.25799999999799</v>
+        <v>741.48799999999926</v>
       </c>
       <c r="E40" s="5">
-        <v>2012.7680000000009</v>
+        <v>2011.226000000001</v>
       </c>
       <c r="F40" s="5">
-        <v>1436.3310000000008</v>
+        <v>1436.3260000000009</v>
       </c>
       <c r="G40" s="5">
-        <v>1241</v>
+        <v>1254.0259999999994</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -1361,17 +3753,17 @@
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5">
-        <v>280.52</v>
+        <v>280.51999999999992</v>
       </c>
       <c r="D41" s="5">
-        <v>215.55400000000034</v>
+        <v>216.56600000000026</v>
       </c>
       <c r="E41" s="5"/>
       <c r="F41" s="5">
-        <v>1359.8640000000007</v>
+        <v>1359.8580000000006</v>
       </c>
       <c r="G41" s="5">
-        <v>436.9920000000003</v>
+        <v>437.1580000000003</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -1385,16 +3777,16 @@
         <v>323.86700000000013</v>
       </c>
       <c r="D42" s="5">
-        <v>269.91800000000012</v>
+        <v>276.27300000000025</v>
       </c>
       <c r="E42" s="5">
         <v>1431.5970000000013</v>
       </c>
       <c r="F42" s="5">
-        <v>2637.4110000000014</v>
+        <v>2637.409000000001</v>
       </c>
       <c r="G42" s="5">
-        <v>685.4609999999999</v>
+        <v>697.98299999999927</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -1406,14 +3798,14 @@
         <v>400.87399999999985</v>
       </c>
       <c r="D43" s="5">
-        <v>324.15899999999982</v>
+        <v>324.66599999999994</v>
       </c>
       <c r="E43" s="5"/>
       <c r="F43" s="5">
-        <v>1580.8009999999999</v>
+        <v>1580.7979999999998</v>
       </c>
       <c r="G43" s="5">
-        <v>484.9379999999997</v>
+        <v>486.27199999999965</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -1427,16 +3819,16 @@
         <v>639.87699999999984</v>
       </c>
       <c r="D44" s="5">
-        <v>1292.209999999998</v>
+        <v>1389.9319999999943</v>
       </c>
       <c r="E44" s="5">
-        <v>2546.2839999999974</v>
+        <v>2546.2829999999972</v>
       </c>
       <c r="F44" s="5">
-        <v>4787.2390000000005</v>
+        <v>4787.2350000000015</v>
       </c>
       <c r="G44" s="5">
-        <v>3787.7049999999927</v>
+        <v>3702.9979999999896</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -1448,14 +3840,14 @@
         <v>120.084</v>
       </c>
       <c r="D45" s="5">
-        <v>89.715000000000074</v>
+        <v>87.606000000000051</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="5">
-        <v>705.34199999999964</v>
+        <v>705.34099999999955</v>
       </c>
       <c r="G45" s="5">
-        <v>197.66199999999992</v>
+        <v>196.78200000000001</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -1469,16 +3861,16 @@
         <v>86.782999999999987</v>
       </c>
       <c r="D46" s="5">
-        <v>314.17399999999975</v>
+        <v>311.57399999999973</v>
       </c>
       <c r="E46" s="5">
-        <v>711.18399999999974</v>
+        <v>711.1819999999999</v>
       </c>
       <c r="F46" s="5">
-        <v>152.91600000000003</v>
+        <v>152.91700000000003</v>
       </c>
       <c r="G46" s="5">
-        <v>209.86700000000002</v>
+        <v>209.88200000000001</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -1497,7 +3889,7 @@
       </c>
       <c r="F47" s="5"/>
       <c r="G47" s="5">
-        <v>19.446999999999999</v>
+        <v>19.421999999999997</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -1512,11 +3904,11 @@
         <v>211.47</v>
       </c>
       <c r="E48" s="5">
-        <v>393.56100000000026</v>
+        <v>393.5420000000002</v>
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5">
-        <v>123.062</v>
+        <v>123.05900000000003</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -1530,16 +3922,16 @@
         <v>36.238999999999997</v>
       </c>
       <c r="D49" s="5">
-        <v>375.54700000000093</v>
+        <v>356.44799999999947</v>
       </c>
       <c r="E49" s="5">
-        <v>3043.6730000000002</v>
+        <v>3043.6679999999992</v>
       </c>
       <c r="F49" s="5">
-        <v>173.52500000000006</v>
+        <v>173.52000000000007</v>
       </c>
       <c r="G49" s="5">
-        <v>666.88</v>
+        <v>666.43700000000047</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -1548,17 +3940,17 @@
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5">
-        <v>278.16900000000004</v>
+        <v>278.16899999999998</v>
       </c>
       <c r="D50" s="5">
-        <v>137.61300000000014</v>
+        <v>143.56500000000017</v>
       </c>
       <c r="E50" s="5"/>
       <c r="F50" s="5">
-        <v>1606.5699999999997</v>
+        <v>1606.5689999999997</v>
       </c>
       <c r="G50" s="5">
-        <v>410.59999999999962</v>
+        <v>411.92399999999964</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -1572,16 +3964,16 @@
         <v>150.04500000000002</v>
       </c>
       <c r="D51" s="5">
-        <v>391.92500000000041</v>
+        <v>391.0770000000004</v>
       </c>
       <c r="E51" s="5">
-        <v>410.10200000000003</v>
+        <v>410.10100000000006</v>
       </c>
       <c r="F51" s="5">
-        <v>943.93500000000006</v>
+        <v>943.93400000000008</v>
       </c>
       <c r="G51" s="5">
-        <v>825.27499999999964</v>
+        <v>827.21100000000069</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
@@ -1593,14 +3985,14 @@
         <v>75.313999999999979</v>
       </c>
       <c r="D52" s="5">
-        <v>164.57900000000004</v>
+        <v>161.52499999999995</v>
       </c>
       <c r="E52" s="5"/>
       <c r="F52" s="5">
-        <v>221.28700000000001</v>
+        <v>221.286</v>
       </c>
       <c r="G52" s="5">
-        <v>311.69100000000003</v>
+        <v>311.6099999999999</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -1617,13 +4009,13 @@
         <v>61.239000000000011</v>
       </c>
       <c r="E53" s="5">
-        <v>487.45499999999998</v>
+        <v>487.45300000000003</v>
       </c>
       <c r="F53" s="5">
         <v>10.33</v>
       </c>
       <c r="G53" s="5">
-        <v>103.13600000000001</v>
+        <v>103.13399999999999</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
@@ -1638,7 +4030,7 @@
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
       <c r="G54" s="5">
-        <v>85.799000000000007</v>
+        <v>85.79</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -1650,14 +4042,14 @@
         <v>298.46600000000018</v>
       </c>
       <c r="D55" s="5">
-        <v>413.72700000000032</v>
+        <v>416.60000000000042</v>
       </c>
       <c r="E55" s="5"/>
       <c r="F55" s="5">
-        <v>1376.8520000000003</v>
+        <v>1376.8530000000003</v>
       </c>
       <c r="G55" s="5">
-        <v>585.55900000000042</v>
+        <v>587.65500000000077</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -1672,7 +4064,7 @@
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
       <c r="G56" s="5">
-        <v>229.50100000000006</v>
+        <v>229.49700000000004</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -1688,10 +4080,10 @@
       </c>
       <c r="E57" s="5"/>
       <c r="F57" s="5">
-        <v>2890.5539999999992</v>
+        <v>2890.5499999999997</v>
       </c>
       <c r="G57" s="5">
-        <v>1782.7169999999976</v>
+        <v>1787.0630000000017</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -1705,16 +4097,16 @@
         <v>48.161999999999999</v>
       </c>
       <c r="D58" s="5">
-        <v>109.45999999999994</v>
+        <v>111.04599999999995</v>
       </c>
       <c r="E58" s="5">
-        <v>1210.3590000000002</v>
+        <v>1210.3540000000005</v>
       </c>
       <c r="F58" s="5">
-        <v>119.791</v>
+        <v>119.789</v>
       </c>
       <c r="G58" s="5">
-        <v>168.16300000000004</v>
+        <v>170.77000000000004</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
@@ -1730,19 +4122,1192 @@
       </c>
       <c r="E59" s="5"/>
       <c r="F59" s="5">
-        <v>130.33800000000002</v>
+        <v>130.33600000000001</v>
       </c>
       <c r="G59" s="5">
-        <v>227.96200000000005</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>64</v>
+        <v>227.95900000000009</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49AA68F6-60B8-024F-8810-AB038083B23E}">
+  <dimension ref="A1:G59"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" customWidth="1"/>
+    <col min="5" max="5" width="33" customWidth="1"/>
+    <col min="6" max="6" width="35.33203125" customWidth="1"/>
+    <col min="7" max="7" width="33.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+      <c r="A1" s="7"/>
+      <c r="B1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8">
+        <v>953.33900000000062</v>
+      </c>
+      <c r="C2" s="8">
+        <v>128.57999999999998</v>
+      </c>
+      <c r="D2" s="8">
+        <v>836.89299999999912</v>
+      </c>
+      <c r="E2" s="8">
+        <v>7930.3680000000004</v>
+      </c>
+      <c r="F2" s="8">
+        <v>786.41199999999981</v>
+      </c>
+      <c r="G2" s="8">
+        <v>2158.7280000000032</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8">
+        <v>53.007999999999996</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8">
+        <v>27.364999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8">
+        <v>204.69300000000007</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8">
+        <v>233.10299999999984</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8">
+        <v>15.105999999999998</v>
+      </c>
+      <c r="D5" s="8">
+        <v>316.94700000000006</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8">
+        <v>34.900999999999996</v>
+      </c>
+      <c r="G5" s="8">
+        <v>823.68299999999931</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8">
+        <v>97.64</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8">
+        <v>104.50999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8">
+        <v>138.54800000000006</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8">
+        <v>92.697999999999993</v>
+      </c>
+      <c r="E7" s="8">
+        <v>377.52600000000007</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8">
+        <v>103.69499999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="8">
+        <v>362.88599999999991</v>
+      </c>
+      <c r="C8" s="8">
+        <v>249.65800000000002</v>
+      </c>
+      <c r="D8" s="8">
+        <v>753.03599999999881</v>
+      </c>
+      <c r="E8" s="8">
+        <v>2767.4289999999974</v>
+      </c>
+      <c r="F8" s="8">
+        <v>1945.7350000000015</v>
+      </c>
+      <c r="G8" s="8">
+        <v>1734.4099999999967</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8">
+        <v>210.44300000000007</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8">
+        <v>168.83600000000007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8">
+        <v>79.635999999999996</v>
+      </c>
+      <c r="D10" s="8">
+        <v>217.69599999999988</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8">
+        <v>413.81</v>
+      </c>
+      <c r="G10" s="8">
+        <v>392.84499999999974</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="8">
+        <v>264.63599999999997</v>
+      </c>
+      <c r="C11" s="8">
+        <v>381.97599999999971</v>
+      </c>
+      <c r="D11" s="8">
+        <v>792.27299999999934</v>
+      </c>
+      <c r="E11" s="8">
+        <v>946.8130000000001</v>
+      </c>
+      <c r="F11" s="8">
+        <v>2068.2869999999989</v>
+      </c>
+      <c r="G11" s="8">
+        <v>1255.3139999999987</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8">
+        <v>115.28399999999999</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8">
+        <v>34.054000000000009</v>
+      </c>
+      <c r="E12" s="8">
+        <v>288.63200000000006</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8">
+        <v>46.038999999999994</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8">
+        <v>655.63000000000022</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8">
+        <v>743.72799999999972</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="8">
+        <v>375.74000000000007</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8">
+        <v>678.86699999999939</v>
+      </c>
+      <c r="E14" s="8">
+        <v>570.30900000000008</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8">
+        <v>729.43900000000008</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8">
+        <v>494.03100000000006</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8">
+        <v>340.28700000000021</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="8">
+        <v>387.34000000000003</v>
+      </c>
+      <c r="C16" s="8">
+        <v>759.78200000000015</v>
+      </c>
+      <c r="D16" s="8">
+        <v>1282.1849999999997</v>
+      </c>
+      <c r="E16" s="8">
+        <v>1344.2920000000004</v>
+      </c>
+      <c r="F16" s="8">
+        <v>2405.3740000000003</v>
+      </c>
+      <c r="G16" s="8">
+        <v>1894.1219999999978</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="8">
+        <v>106.95599999999999</v>
+      </c>
+      <c r="C17" s="8">
+        <v>65.923000000000016</v>
+      </c>
+      <c r="D17" s="8">
+        <v>191.55800000000011</v>
+      </c>
+      <c r="E17" s="8">
+        <v>355.72500000000002</v>
+      </c>
+      <c r="F17" s="8">
+        <v>202.48700000000002</v>
+      </c>
+      <c r="G17" s="8">
+        <v>253.375</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8">
+        <v>149.95699999999991</v>
+      </c>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8">
+        <v>214.08000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8">
+        <v>400.71600000000024</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8">
+        <v>228.511</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="8">
+        <v>2759.202000000002</v>
+      </c>
+      <c r="C20" s="8">
+        <v>1709.853999999998</v>
+      </c>
+      <c r="D20" s="8">
+        <v>7488.8019999999369</v>
+      </c>
+      <c r="E20" s="8">
+        <v>23603.734999999997</v>
+      </c>
+      <c r="F20" s="8">
+        <v>13572.466999999997</v>
+      </c>
+      <c r="G20" s="8">
+        <v>19093.756999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8">
+        <v>123.24600000000002</v>
+      </c>
+      <c r="D21" s="8">
+        <v>182.68100000000007</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8">
+        <v>690.00199999999995</v>
+      </c>
+      <c r="G21" s="8">
+        <v>359.91500000000036</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="8">
+        <v>27.192</v>
+      </c>
+      <c r="C22" s="8">
+        <v>229.75199999999995</v>
+      </c>
+      <c r="D22" s="8">
+        <v>92.374000000000024</v>
+      </c>
+      <c r="E22" s="8">
+        <v>175.50500000000002</v>
+      </c>
+      <c r="F22" s="8">
+        <v>1502.0050000000003</v>
+      </c>
+      <c r="G22" s="8">
+        <v>218.84400000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8">
+        <v>201.43399999999988</v>
+      </c>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8">
+        <v>90.385999999999939</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8">
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="D24" s="8">
+        <v>379.71199999999988</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8">
+        <v>1.448</v>
+      </c>
+      <c r="G24" s="8">
+        <v>536.66999999999985</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="8">
+        <v>128.54799999999994</v>
+      </c>
+      <c r="C25" s="8">
+        <v>161.506</v>
+      </c>
+      <c r="D25" s="8">
+        <v>382.67999999999972</v>
+      </c>
+      <c r="E25" s="8">
+        <v>393.05999999999995</v>
+      </c>
+      <c r="F25" s="8">
+        <v>687.47699999999986</v>
+      </c>
+      <c r="G25" s="8">
+        <v>636.16999999999973</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8">
+        <v>258.86199999999997</v>
+      </c>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8">
+        <v>53.625999999999983</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8">
+        <v>428.38599999999997</v>
+      </c>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8">
+        <v>212.42299999999989</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8">
+        <v>494.19700000000012</v>
+      </c>
+      <c r="D28" s="8">
+        <v>243.42499999999993</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8">
+        <v>1591.6020000000001</v>
+      </c>
+      <c r="G28" s="8">
+        <v>721.53300000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8">
+        <v>39.534999999999989</v>
+      </c>
+      <c r="D29" s="8">
+        <v>97.562000000000012</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8">
+        <v>182.16900000000004</v>
+      </c>
+      <c r="G29" s="8">
+        <v>298.35000000000008</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="8">
+        <v>147.68199999999996</v>
+      </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8">
+        <v>143.74600000000007</v>
+      </c>
+      <c r="E30" s="8">
+        <v>320.73000000000008</v>
+      </c>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8">
+        <v>299.1880000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="8">
+        <v>755.87299999999982</v>
+      </c>
+      <c r="C31" s="8">
+        <v>900.91899999999998</v>
+      </c>
+      <c r="D31" s="8">
+        <v>3170.0179999999955</v>
+      </c>
+      <c r="E31" s="8">
+        <v>6657.3329999999969</v>
+      </c>
+      <c r="F31" s="8">
+        <v>6060.3620000000055</v>
+      </c>
+      <c r="G31" s="8">
+        <v>7690.7980000000107</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="8">
+        <v>325.46100000000007</v>
+      </c>
+      <c r="C32" s="8">
+        <v>43.051000000000009</v>
+      </c>
+      <c r="D32" s="8">
+        <v>203.20000000000005</v>
+      </c>
+      <c r="E32" s="8">
+        <v>1391.7590000000002</v>
+      </c>
+      <c r="F32" s="8">
+        <v>250.57099999999994</v>
+      </c>
+      <c r="G32" s="8">
+        <v>465.01600000000008</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="8">
+        <v>1302.9670000000003</v>
+      </c>
+      <c r="C34" s="8">
+        <v>366.99099999999993</v>
+      </c>
+      <c r="D34" s="8">
+        <v>964.74800000000062</v>
+      </c>
+      <c r="E34" s="8">
+        <v>7035.6240000000007</v>
+      </c>
+      <c r="F34" s="8">
+        <v>2931.7489999999993</v>
+      </c>
+      <c r="G34" s="8">
+        <v>2265.1389999999997</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="8">
+        <v>354.60000000000008</v>
+      </c>
+      <c r="C35" s="8">
+        <v>390.05900000000025</v>
+      </c>
+      <c r="D35" s="8">
+        <v>1021.3449999999982</v>
+      </c>
+      <c r="E35" s="8">
+        <v>2472.2089999999998</v>
+      </c>
+      <c r="F35" s="8">
+        <v>2888.7539999999985</v>
+      </c>
+      <c r="G35" s="8">
+        <v>2684.3000000000034</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8">
+        <v>25.457000000000001</v>
+      </c>
+      <c r="D36" s="8">
+        <v>96.586999999999961</v>
+      </c>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8">
+        <v>122.58799999999999</v>
+      </c>
+      <c r="G36" s="8">
+        <v>245.59299999999996</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="8">
+        <v>1976.970999999998</v>
+      </c>
+      <c r="C37" s="8">
+        <v>383.47500000000019</v>
+      </c>
+      <c r="D37" s="8">
+        <v>1666.2289999999978</v>
+      </c>
+      <c r="E37" s="8">
+        <v>8520.2630000000026</v>
+      </c>
+      <c r="F37" s="8">
+        <v>2657.2849999999999</v>
+      </c>
+      <c r="G37" s="8">
+        <v>3057.3530000000055</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="8">
+        <v>1686.7720000000004</v>
+      </c>
+      <c r="C38" s="8">
+        <v>702.87399999999968</v>
+      </c>
+      <c r="D38" s="8">
+        <v>1189.8429999999978</v>
+      </c>
+      <c r="E38" s="8">
+        <v>11580.371000000017</v>
+      </c>
+      <c r="F38" s="8">
+        <v>4741.8629999999948</v>
+      </c>
+      <c r="G38" s="8">
+        <v>3139.0850000000069</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="8">
+        <v>63.292000000000002</v>
+      </c>
+      <c r="C39" s="8">
+        <v>76.735000000000014</v>
+      </c>
+      <c r="D39" s="8">
+        <v>400.93799999999999</v>
+      </c>
+      <c r="E39" s="8">
+        <v>466.22399999999999</v>
+      </c>
+      <c r="F39" s="8">
+        <v>720.48700000000031</v>
+      </c>
+      <c r="G39" s="8">
+        <v>981.24499999999944</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="8">
+        <v>402.23999999999984</v>
+      </c>
+      <c r="C40" s="8">
+        <v>248.17499999999993</v>
+      </c>
+      <c r="D40" s="8">
+        <v>755.25799999999799</v>
+      </c>
+      <c r="E40" s="8">
+        <v>2012.7680000000009</v>
+      </c>
+      <c r="F40" s="8">
+        <v>1436.3310000000008</v>
+      </c>
+      <c r="G40" s="8">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8">
+        <v>280.52</v>
+      </c>
+      <c r="D41" s="8">
+        <v>215.55400000000034</v>
+      </c>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8">
+        <v>1359.8640000000007</v>
+      </c>
+      <c r="G41" s="8">
+        <v>436.9920000000003</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="8">
+        <v>246.14499999999995</v>
+      </c>
+      <c r="C42" s="8">
+        <v>323.86700000000013</v>
+      </c>
+      <c r="D42" s="8">
+        <v>269.91800000000012</v>
+      </c>
+      <c r="E42" s="8">
+        <v>1431.5970000000013</v>
+      </c>
+      <c r="F42" s="8">
+        <v>2637.4110000000014</v>
+      </c>
+      <c r="G42" s="8">
+        <v>685.4609999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8">
+        <v>400.87399999999985</v>
+      </c>
+      <c r="D43" s="8">
+        <v>324.15899999999982</v>
+      </c>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8">
+        <v>1580.8009999999999</v>
+      </c>
+      <c r="G43" s="8">
+        <v>484.9379999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="8">
+        <v>340.99099999999981</v>
+      </c>
+      <c r="C44" s="8">
+        <v>639.87699999999984</v>
+      </c>
+      <c r="D44" s="8">
+        <v>1292.209999999998</v>
+      </c>
+      <c r="E44" s="8">
+        <v>2546.2839999999974</v>
+      </c>
+      <c r="F44" s="8">
+        <v>4787.2390000000005</v>
+      </c>
+      <c r="G44" s="8">
+        <v>3787.7049999999927</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8">
+        <v>120.084</v>
+      </c>
+      <c r="D45" s="8">
+        <v>89.715000000000074</v>
+      </c>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8">
+        <v>705.34199999999964</v>
+      </c>
+      <c r="G45" s="8">
+        <v>197.66199999999992</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46" s="8">
+        <v>341.29100000000011</v>
+      </c>
+      <c r="C46" s="8">
+        <v>86.782999999999987</v>
+      </c>
+      <c r="D46" s="8">
+        <v>314.17399999999975</v>
+      </c>
+      <c r="E46" s="8">
+        <v>711.18399999999974</v>
+      </c>
+      <c r="F46" s="8">
+        <v>152.91600000000003</v>
+      </c>
+      <c r="G46" s="8">
+        <v>209.86700000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" s="8">
+        <v>15.548</v>
+      </c>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8">
+        <v>18.962000000000003</v>
+      </c>
+      <c r="E47" s="8">
+        <v>44.122999999999998</v>
+      </c>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8">
+        <v>19.446999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" s="8">
+        <v>295.54000000000008</v>
+      </c>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8">
+        <v>211.47</v>
+      </c>
+      <c r="E48" s="8">
+        <v>393.56100000000026</v>
+      </c>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8">
+        <v>123.062</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" s="8">
+        <v>463.92699999999996</v>
+      </c>
+      <c r="C49" s="8">
+        <v>36.238999999999997</v>
+      </c>
+      <c r="D49" s="8">
+        <v>375.54700000000093</v>
+      </c>
+      <c r="E49" s="8">
+        <v>3043.6730000000002</v>
+      </c>
+      <c r="F49" s="8">
+        <v>173.52500000000006</v>
+      </c>
+      <c r="G49" s="8">
+        <v>666.88</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8">
+        <v>278.16900000000004</v>
+      </c>
+      <c r="D50" s="8">
+        <v>137.61300000000014</v>
+      </c>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8">
+        <v>1606.5699999999997</v>
+      </c>
+      <c r="G50" s="8">
+        <v>410.59999999999962</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51" s="8">
+        <v>114.33300000000001</v>
+      </c>
+      <c r="C51" s="8">
+        <v>150.04500000000002</v>
+      </c>
+      <c r="D51" s="8">
+        <v>391.92500000000041</v>
+      </c>
+      <c r="E51" s="8">
+        <v>410.10200000000003</v>
+      </c>
+      <c r="F51" s="8">
+        <v>943.93500000000006</v>
+      </c>
+      <c r="G51" s="8">
+        <v>825.27499999999964</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8">
+        <v>75.313999999999979</v>
+      </c>
+      <c r="D52" s="8">
+        <v>164.57900000000004</v>
+      </c>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8">
+        <v>221.28700000000001</v>
+      </c>
+      <c r="G52" s="8">
+        <v>311.69100000000003</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53" s="8">
+        <v>169.57699999999997</v>
+      </c>
+      <c r="C53" s="8">
+        <v>6.2919999999999998</v>
+      </c>
+      <c r="D53" s="8">
+        <v>61.239000000000011</v>
+      </c>
+      <c r="E53" s="8">
+        <v>487.45499999999998</v>
+      </c>
+      <c r="F53" s="8">
+        <v>10.33</v>
+      </c>
+      <c r="G53" s="8">
+        <v>103.13600000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8">
+        <v>151.28500000000003</v>
+      </c>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8">
+        <v>85.799000000000007</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8">
+        <v>298.46600000000018</v>
+      </c>
+      <c r="D55" s="8">
+        <v>413.72700000000032</v>
+      </c>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8">
+        <v>1376.8520000000003</v>
+      </c>
+      <c r="G55" s="8">
+        <v>585.55900000000042</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8">
+        <v>177.82599999999996</v>
+      </c>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="8">
+        <v>229.50100000000006</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B57" s="8"/>
+      <c r="C57" s="8">
+        <v>431.38199999999989</v>
+      </c>
+      <c r="D57" s="8">
+        <v>878.83599999999933</v>
+      </c>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8">
+        <v>2890.5539999999992</v>
+      </c>
+      <c r="G57" s="8">
+        <v>1782.7169999999976</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B58" s="8">
+        <v>302.04700000000003</v>
+      </c>
+      <c r="C58" s="8">
+        <v>48.161999999999999</v>
+      </c>
+      <c r="D58" s="8">
+        <v>109.45999999999994</v>
+      </c>
+      <c r="E58" s="8">
+        <v>1210.3590000000002</v>
+      </c>
+      <c r="F58" s="8">
+        <v>119.791</v>
+      </c>
+      <c r="G58" s="8">
+        <v>168.16300000000004</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B59" s="8"/>
+      <c r="C59" s="8">
+        <v>48.127999999999993</v>
+      </c>
+      <c r="D59" s="8">
+        <v>103.636</v>
+      </c>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8">
+        <v>130.33800000000002</v>
+      </c>
+      <c r="G59" s="8">
+        <v>227.96200000000005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>